<commit_message>
Add persistence: load team budgets and RTM status from Excel on startup
</commit_message>
<xml_diff>
--- a/data/auction_data.xlsx
+++ b/data/auction_data.xlsx
@@ -792,7 +792,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -831,6 +831,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add logging and regenerate Excel with correct schema (RTM column)
</commit_message>
<xml_diff>
--- a/data/auction_data.xlsx
+++ b/data/auction_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Base Price</t>
   </si>
   <si>
+    <t>Franchise ID</t>
+  </si>
+  <si>
     <t>Virat Kohli</t>
   </si>
   <si>
@@ -111,6 +114,9 @@
   </si>
   <si>
     <t>Final Price</t>
+  </si>
+  <si>
+    <t>RTM Used</t>
   </si>
 </sst>
 </file>
@@ -487,16 +493,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,296 +515,359 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -807,30 +876,34 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Excel save issues: improve error handling, remove lock files, add debug logging
</commit_message>
<xml_diff>
--- a/data/auction_data.xlsx
+++ b/data/auction_data.xlsx
@@ -861,7 +861,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -904,6 +904,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add frontend and backend logging for team player fetch debugging
</commit_message>
<xml_diff>
--- a/data/auction_data.xlsx
+++ b/data/auction_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>RTM Used</t>
+  </si>
+  <si>
+    <t>Mumbai Indians</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Chennai Super Kings</t>
+  </si>
+  <si>
+    <t>Royal Challengers Bangalore</t>
   </si>
 </sst>
 </file>
@@ -867,7 +879,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -902,6 +914,75 @@
         <v>34</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>